<commit_message>
added vertical and horizontal header
</commit_message>
<xml_diff>
--- a/src/test/java/com/catapult/excel/analyzer/format2.xlsx
+++ b/src/test/java/com/catapult/excel/analyzer/format2.xlsx
@@ -7629,8 +7629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DY3787"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U17" sqref="U17"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="BD13" sqref="BD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -7676,9 +7676,8 @@
     <col min="48" max="48" width="15" style="7" hidden="1" customWidth="1"/>
     <col min="49" max="51" width="9.7109375" style="7" customWidth="1"/>
     <col min="52" max="52" width="16.140625" style="7" hidden="1" customWidth="1"/>
-    <col min="53" max="55" width="14.7109375" style="7" customWidth="1"/>
-    <col min="56" max="56" width="14.7109375" style="7" hidden="1" customWidth="1"/>
-    <col min="57" max="57" width="14.7109375" style="62" hidden="1" customWidth="1"/>
+    <col min="53" max="56" width="14.7109375" style="7" customWidth="1"/>
+    <col min="57" max="57" width="14.7109375" style="62" customWidth="1"/>
     <col min="58" max="58" width="3.7109375" style="62" customWidth="1"/>
     <col min="59" max="70" width="14.7109375" style="62" customWidth="1"/>
     <col min="71" max="116" width="14.7109375" style="8" customWidth="1"/>

</xml_diff>